<commit_message>
The GSR data and the HR data are analyzed and compiled.
</commit_message>
<xml_diff>
--- a/Yoda Behavior Analysis_Conversion.xlsx
+++ b/Yoda Behavior Analysis_Conversion.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="155">
   <si>
     <t xml:space="preserve">Participant</t>
   </si>
@@ -294,9 +294,6 @@
   </si>
   <si>
     <t xml:space="preserve">Yoda 058 - Yoda 058 - 2018-09-12 18-57-43</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1?</t>
   </si>
   <si>
     <t xml:space="preserve">a little sleepy 21:21, 31:12.almost fell asleep 33:10, 35:35</t>
@@ -593,7 +590,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -616,6 +613,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF62A73B"/>
         <bgColor rgb="FF808000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF200"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -667,7 +670,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -700,10 +703,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -721,6 +720,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -748,7 +755,7 @@
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFFF200"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
@@ -811,34 +818,34 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="AJ13" activeCellId="1" sqref="AJ12 AJ13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="K58" activeCellId="0" sqref="K58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="62.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="7.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="9.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="20.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="7.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="6.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="8.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="6.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="11.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="10.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="6.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="6.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="9.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="7.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="9.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="10.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="12.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="10.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="6.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="6.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="11.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="7.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="7.84"/>
@@ -1062,7 +1069,7 @@
         <v>1</v>
       </c>
       <c r="K3" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L3" s="7"/>
       <c r="M3" s="7"/>
@@ -1367,7 +1374,7 @@
       <c r="E7" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F7" s="8" t="n">
+      <c r="F7" s="1" t="n">
         <v>0</v>
       </c>
       <c r="G7" s="1" t="n">
@@ -1400,7 +1407,7 @@
       <c r="P7" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q7" s="9" t="n">
+      <c r="Q7" s="8" t="n">
         <v>1</v>
       </c>
       <c r="R7" s="1" t="n">
@@ -1445,7 +1452,7 @@
       <c r="AE7" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AF7" s="8" t="n">
+      <c r="AF7" s="1" t="n">
         <v>1</v>
       </c>
       <c r="AG7" s="1" t="s">
@@ -1489,7 +1496,7 @@
       <c r="E8" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F8" s="8" t="n">
+      <c r="F8" s="1" t="n">
         <v>0</v>
       </c>
       <c r="G8" s="1" t="n">
@@ -1505,7 +1512,7 @@
         <v>0</v>
       </c>
       <c r="K8" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L8" s="1" t="n">
         <v>0</v>
@@ -1522,7 +1529,7 @@
       <c r="P8" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q8" s="9" t="n">
+      <c r="Q8" s="8" t="n">
         <v>0</v>
       </c>
       <c r="R8" s="1" t="n">
@@ -1605,7 +1612,7 @@
       <c r="C9" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D9" s="9" t="n">
+      <c r="D9" s="8" t="n">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="n">
@@ -1644,19 +1651,19 @@
       <c r="P9" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q9" s="9" t="n">
+      <c r="Q9" s="8" t="n">
         <v>1</v>
       </c>
       <c r="R9" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="S9" s="10" t="n">
+      <c r="S9" s="9" t="n">
         <v>0</v>
       </c>
       <c r="T9" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="U9" s="10" t="n">
+      <c r="U9" s="9" t="n">
         <v>0</v>
       </c>
       <c r="V9" s="1" t="n">
@@ -1665,19 +1672,19 @@
       <c r="W9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="X9" s="10" t="n">
+      <c r="X9" s="9" t="n">
         <v>1</v>
       </c>
       <c r="Y9" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Z9" s="10" t="n">
+      <c r="Z9" s="9" t="n">
         <v>0</v>
       </c>
       <c r="AA9" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AB9" s="10" t="n">
+      <c r="AB9" s="9" t="n">
         <v>0</v>
       </c>
       <c r="AC9" s="1" t="n">
@@ -1686,7 +1693,7 @@
       <c r="AD9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AE9" s="10" t="n">
+      <c r="AE9" s="9" t="n">
         <v>0</v>
       </c>
       <c r="AF9" s="1" t="n">
@@ -1695,7 +1702,7 @@
       <c r="AG9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AH9" s="10" t="n">
+      <c r="AH9" s="9" t="n">
         <v>0</v>
       </c>
       <c r="AI9" s="1" t="n">
@@ -1704,7 +1711,7 @@
       <c r="AJ9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AK9" s="10" t="n">
+      <c r="AK9" s="9" t="n">
         <v>0</v>
       </c>
       <c r="AL9" s="1" t="n">
@@ -1787,7 +1794,7 @@
       <c r="W10" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="X10" s="10" t="n">
+      <c r="X10" s="9" t="n">
         <v>0</v>
       </c>
       <c r="Y10" s="1" t="n">
@@ -1871,7 +1878,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L11" s="1" t="n">
         <v>0</v>
@@ -1909,7 +1916,7 @@
       <c r="W11" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="X11" s="9" t="n">
+      <c r="X11" s="8" t="n">
         <v>0</v>
       </c>
       <c r="Y11" s="1" t="n">
@@ -1993,7 +2000,7 @@
         <v>0</v>
       </c>
       <c r="K12" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L12" s="1" t="n">
         <v>0</v>
@@ -2031,7 +2038,7 @@
       <c r="W12" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="X12" s="9" t="n">
+      <c r="X12" s="8" t="n">
         <v>0</v>
       </c>
       <c r="Y12" s="1" t="n">
@@ -2067,7 +2074,7 @@
       <c r="AI12" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AJ12" s="8" t="n">
+      <c r="AJ12" s="1" t="n">
         <v>1</v>
       </c>
       <c r="AK12" s="1" t="n">
@@ -2189,7 +2196,7 @@
       <c r="AI13" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AJ13" s="8" t="n">
+      <c r="AJ13" s="1" t="n">
         <v>0</v>
       </c>
       <c r="AK13" s="1" t="n">
@@ -2305,7 +2312,7 @@
       <c r="AG14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AH14" s="10" t="n">
+      <c r="AH14" s="9" t="n">
         <v>0</v>
       </c>
       <c r="AI14" s="1" t="n">
@@ -2359,7 +2366,7 @@
         <v>0</v>
       </c>
       <c r="K15" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L15" s="7"/>
       <c r="M15" s="7"/>
@@ -2425,7 +2432,7 @@
         <v>0</v>
       </c>
       <c r="K16" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L16" s="1" t="n">
         <v>0</v>
@@ -2547,7 +2554,7 @@
         <v>0</v>
       </c>
       <c r="K17" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L17" s="1" t="n">
         <v>1</v>
@@ -2656,7 +2663,7 @@
       <c r="F18" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G18" s="10" t="n">
+      <c r="G18" s="9" t="n">
         <v>0</v>
       </c>
       <c r="H18" s="1" t="n">
@@ -2665,19 +2672,19 @@
       <c r="I18" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="J18" s="10" t="n">
+      <c r="J18" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K18" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L18" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" s="9" t="n">
         <v>0</v>
       </c>
       <c r="M18" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="N18" s="10" t="n">
+      <c r="N18" s="9" t="n">
         <v>0</v>
       </c>
       <c r="O18" s="1" t="n">
@@ -2692,13 +2699,13 @@
       <c r="R18" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="S18" s="10" t="n">
+      <c r="S18" s="9" t="n">
         <v>0</v>
       </c>
       <c r="T18" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="U18" s="10" t="n">
+      <c r="U18" s="9" t="n">
         <v>0</v>
       </c>
       <c r="V18" s="1" t="n">
@@ -2713,13 +2720,13 @@
       <c r="Y18" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Z18" s="10" t="n">
+      <c r="Z18" s="9" t="n">
         <v>0</v>
       </c>
       <c r="AA18" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AB18" s="10" t="n">
+      <c r="AB18" s="9" t="n">
         <v>0</v>
       </c>
       <c r="AC18" s="1" t="n">
@@ -2746,7 +2753,7 @@
       <c r="AJ18" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AK18" s="10" t="n">
+      <c r="AK18" s="9" t="n">
         <v>0</v>
       </c>
       <c r="AL18" s="1" t="n">
@@ -2791,7 +2798,7 @@
         <v>0</v>
       </c>
       <c r="K19" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L19" s="1" t="n">
         <v>0</v>
@@ -2829,7 +2836,7 @@
       <c r="W19" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="X19" s="9" t="n">
+      <c r="X19" s="8" t="n">
         <v>0</v>
       </c>
       <c r="Y19" s="1" t="n">
@@ -2877,7 +2884,7 @@
       <c r="AM19" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AN19" s="9" t="s">
+      <c r="AN19" s="8" t="s">
         <v>57</v>
       </c>
     </row>
@@ -2951,7 +2958,7 @@
       <c r="W20" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="X20" s="9" t="n">
+      <c r="X20" s="8" t="n">
         <v>0</v>
       </c>
       <c r="Y20" s="1" t="n">
@@ -2981,7 +2988,7 @@
       <c r="AG20" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AH20" s="10" t="n">
+      <c r="AH20" s="9" t="n">
         <v>0</v>
       </c>
       <c r="AI20" s="1" t="n">
@@ -2990,7 +2997,7 @@
       <c r="AJ20" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AK20" s="10" t="n">
+      <c r="AK20" s="9" t="n">
         <v>0</v>
       </c>
       <c r="AL20" s="1" t="n">
@@ -3035,7 +3042,7 @@
         <v>0</v>
       </c>
       <c r="K21" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L21" s="1" t="n">
         <v>0</v>
@@ -3073,7 +3080,7 @@
       <c r="W21" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="X21" s="9" t="n">
+      <c r="X21" s="8" t="n">
         <v>0</v>
       </c>
       <c r="Y21" s="1" t="n">
@@ -3154,7 +3161,7 @@
         <v>1</v>
       </c>
       <c r="K22" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L22" s="1" t="n">
         <v>1</v>
@@ -3276,7 +3283,7 @@
         <v>1</v>
       </c>
       <c r="K23" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L23" s="1" t="n">
         <v>1</v>
@@ -3314,7 +3321,7 @@
       <c r="W23" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="X23" s="9" t="n">
+      <c r="X23" s="8" t="n">
         <v>1</v>
       </c>
       <c r="Y23" s="1" t="n">
@@ -3398,7 +3405,7 @@
         <v>0</v>
       </c>
       <c r="K24" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L24" s="7" t="s">
         <v>66</v>
@@ -3436,7 +3443,7 @@
       <c r="W24" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="X24" s="10" t="n">
+      <c r="X24" s="9" t="n">
         <v>0</v>
       </c>
       <c r="Y24" s="1" t="n">
@@ -3463,11 +3470,11 @@
       <c r="AF24" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AG24" s="11" t="s">
+      <c r="AG24" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="AH24" s="11"/>
-      <c r="AI24" s="11"/>
+      <c r="AH24" s="10"/>
+      <c r="AI24" s="10"/>
       <c r="AJ24" s="1" t="n">
         <v>1</v>
       </c>
@@ -3554,7 +3561,7 @@
       <c r="W25" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="X25" s="9" t="n">
+      <c r="X25" s="8" t="n">
         <v>1</v>
       </c>
       <c r="Y25" s="1" t="n">
@@ -3676,7 +3683,7 @@
       <c r="W26" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="X26" s="9" t="n">
+      <c r="X26" s="8" t="n">
         <v>1</v>
       </c>
       <c r="Y26" s="1" t="n">
@@ -3697,7 +3704,7 @@
       <c r="AD26" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AE26" s="9" t="n">
+      <c r="AE26" s="8" t="n">
         <v>1</v>
       </c>
       <c r="AF26" s="1" t="n">
@@ -3706,7 +3713,7 @@
       <c r="AG26" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AH26" s="9" t="n">
+      <c r="AH26" s="8" t="n">
         <v>1</v>
       </c>
       <c r="AI26" s="1" t="n">
@@ -3715,7 +3722,7 @@
       <c r="AJ26" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AK26" s="10" t="n">
+      <c r="AK26" s="9" t="n">
         <v>0</v>
       </c>
       <c r="AL26" s="1" t="n">
@@ -3760,7 +3767,7 @@
         <v>0</v>
       </c>
       <c r="K27" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L27" s="1" t="n">
         <v>1</v>
@@ -3798,7 +3805,7 @@
       <c r="W27" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="X27" s="9" t="n">
+      <c r="X27" s="8" t="n">
         <v>1</v>
       </c>
       <c r="Y27" s="1" t="n">
@@ -3968,7 +3975,7 @@
       <c r="AM28" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="AMJ28" s="12"/>
+      <c r="AMJ28" s="11"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
@@ -4002,7 +4009,7 @@
         <v>0</v>
       </c>
       <c r="K29" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L29" s="1" t="n">
         <v>0</v>
@@ -4010,7 +4017,7 @@
       <c r="M29" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="N29" s="10" t="n">
+      <c r="N29" s="9" t="n">
         <v>0</v>
       </c>
       <c r="O29" s="1" t="n">
@@ -4040,7 +4047,7 @@
       <c r="W29" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="X29" s="10" t="n">
+      <c r="X29" s="9" t="n">
         <v>0</v>
       </c>
       <c r="Y29" s="1" t="n">
@@ -4052,7 +4059,7 @@
       <c r="AA29" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AB29" s="10" t="n">
+      <c r="AB29" s="9" t="n">
         <v>0</v>
       </c>
       <c r="AC29" s="1" t="s">
@@ -4061,7 +4068,7 @@
       <c r="AD29" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AE29" s="10" t="n">
+      <c r="AE29" s="9" t="n">
         <v>0</v>
       </c>
       <c r="AF29" s="1" t="n">
@@ -4070,7 +4077,7 @@
       <c r="AG29" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AH29" s="10" t="n">
+      <c r="AH29" s="9" t="n">
         <v>0</v>
       </c>
       <c r="AI29" s="1" t="n">
@@ -4162,13 +4169,13 @@
       <c r="W30" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="X30" s="10" t="n">
+      <c r="X30" s="9" t="n">
         <v>0</v>
       </c>
       <c r="Y30" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Z30" s="10" t="n">
+      <c r="Z30" s="9" t="n">
         <v>0</v>
       </c>
       <c r="AA30" s="1" t="n">
@@ -4183,7 +4190,7 @@
       <c r="AD30" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AE30" s="10" t="n">
+      <c r="AE30" s="9" t="n">
         <v>0</v>
       </c>
       <c r="AF30" s="1" t="n">
@@ -4201,7 +4208,7 @@
       <c r="AJ30" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AK30" s="10" t="n">
+      <c r="AK30" s="9" t="n">
         <v>0</v>
       </c>
       <c r="AL30" s="1" t="n">
@@ -4284,7 +4291,7 @@
       <c r="W31" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="X31" s="9" t="n">
+      <c r="X31" s="8" t="n">
         <v>0</v>
       </c>
       <c r="Y31" s="1" t="n">
@@ -4403,7 +4410,7 @@
       <c r="W32" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="X32" s="9" t="n">
+      <c r="X32" s="8" t="n">
         <v>0</v>
       </c>
       <c r="Y32" s="1" t="n">
@@ -4424,8 +4431,8 @@
       <c r="AD32" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AE32" s="1" t="s">
-        <v>91</v>
+      <c r="AE32" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="AF32" s="1" t="n">
         <v>0</v>
@@ -4433,7 +4440,7 @@
       <c r="AG32" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AH32" s="10" t="n">
+      <c r="AH32" s="9" t="n">
         <v>0</v>
       </c>
       <c r="AI32" s="1" t="n">
@@ -4442,7 +4449,7 @@
       <c r="AJ32" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AK32" s="10" t="n">
+      <c r="AK32" s="9" t="n">
         <v>0</v>
       </c>
       <c r="AL32" s="1" t="n">
@@ -4452,7 +4459,7 @@
         <v>1</v>
       </c>
       <c r="AN32" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4460,7 +4467,7 @@
         <v>57</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C33" s="1" t="n">
         <v>1</v>
@@ -4487,7 +4494,7 @@
         <v>0</v>
       </c>
       <c r="K33" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L33" s="1" t="n">
         <v>0</v>
@@ -4525,7 +4532,7 @@
       <c r="W33" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="X33" s="9" t="n">
+      <c r="X33" s="8" t="n">
         <v>0</v>
       </c>
       <c r="Y33" s="1" t="n">
@@ -4574,7 +4581,7 @@
         <v>0</v>
       </c>
       <c r="AN33" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4582,7 +4589,7 @@
         <v>64</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C34" s="1" t="n">
         <v>1</v>
@@ -4696,7 +4703,7 @@
         <v>1</v>
       </c>
       <c r="AN34" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4704,7 +4711,7 @@
         <v>71</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C35" s="1" t="n">
         <v>1</v>
@@ -4727,11 +4734,11 @@
       <c r="I35" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="J35" s="10" t="n">
+      <c r="J35" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K35" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L35" s="1" t="n">
         <v>0</v>
@@ -4769,7 +4776,7 @@
       <c r="W35" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="X35" s="10" t="n">
+      <c r="X35" s="9" t="n">
         <v>0</v>
       </c>
       <c r="Y35" s="1" t="n">
@@ -4781,7 +4788,7 @@
       <c r="AA35" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AB35" s="10" t="n">
+      <c r="AB35" s="9" t="n">
         <v>0</v>
       </c>
       <c r="AC35" s="1" t="n">
@@ -4808,7 +4815,7 @@
       <c r="AJ35" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AK35" s="10" t="n">
+      <c r="AK35" s="9" t="n">
         <v>0</v>
       </c>
       <c r="AL35" s="1" t="n">
@@ -4818,7 +4825,7 @@
         <v>0</v>
       </c>
       <c r="AN35" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4826,7 +4833,7 @@
         <v>69</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C36" s="1" t="n">
         <v>1</v>
@@ -4853,7 +4860,7 @@
         <v>1</v>
       </c>
       <c r="K36" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L36" s="1" t="n">
         <v>1</v>
@@ -4891,7 +4898,7 @@
       <c r="W36" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="X36" s="9" t="n">
+      <c r="X36" s="8" t="n">
         <v>1</v>
       </c>
       <c r="Y36" s="1" t="n">
@@ -4940,7 +4947,7 @@
         <v>1</v>
       </c>
       <c r="AN36" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4948,7 +4955,7 @@
         <v>67</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C37" s="1" t="n">
         <v>1</v>
@@ -5013,7 +5020,7 @@
       <c r="W37" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="X37" s="9" t="n">
+      <c r="X37" s="8" t="n">
         <v>1</v>
       </c>
       <c r="Y37" s="1" t="n">
@@ -5061,8 +5068,8 @@
       <c r="AM37" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AN37" s="9" t="s">
-        <v>102</v>
+      <c r="AN37" s="8" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5070,7 +5077,7 @@
         <v>66</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C38" s="1" t="n">
         <v>1</v>
@@ -5183,8 +5190,8 @@
       <c r="AM38" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AN38" s="13" t="s">
-        <v>104</v>
+      <c r="AN38" s="12" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5192,7 +5199,7 @@
         <v>77</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C39" s="1" t="n">
         <v>1</v>
@@ -5296,7 +5303,7 @@
       <c r="AJ39" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AK39" s="10" t="n">
+      <c r="AK39" s="9" t="n">
         <v>0</v>
       </c>
       <c r="AL39" s="1" t="n">
@@ -5306,7 +5313,7 @@
         <v>0</v>
       </c>
       <c r="AN39" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5314,7 +5321,7 @@
         <v>76</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C40" s="1" t="n">
         <v>1</v>
@@ -5341,7 +5348,7 @@
         <v>0</v>
       </c>
       <c r="K40" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L40" s="1" t="n">
         <v>0</v>
@@ -5379,7 +5386,7 @@
       <c r="W40" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="X40" s="9" t="n">
+      <c r="X40" s="8" t="n">
         <v>0</v>
       </c>
       <c r="Y40" s="1" t="n">
@@ -5428,128 +5435,123 @@
         <v>0</v>
       </c>
       <c r="AN40" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="41" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="13" t="n">
+        <v>80</v>
+      </c>
+      <c r="B41" s="13" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="n">
-        <v>80</v>
-      </c>
-      <c r="B41" s="1" t="s">
+      <c r="C41" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="D41" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="E41" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="G41" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="H41" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I41" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="J41" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K41" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="L41" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="M41" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="N41" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="O41" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="P41" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q41" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="R41" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="S41" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="T41" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="U41" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="V41" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="W41" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="X41" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y41" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z41" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA41" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB41" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC41" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD41" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE41" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF41" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG41" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="AN41" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="C41" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D41" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E41" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F41" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G41" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H41" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I41" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J41" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K41" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L41" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M41" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="N41" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O41" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="P41" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q41" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="R41" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="S41" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="T41" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="U41" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="V41" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="W41" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="X41" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y41" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z41" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA41" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB41" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC41" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD41" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE41" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF41" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG41" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="AH41" s="7"/>
-      <c r="AI41" s="7"/>
-      <c r="AJ41" s="7"/>
-      <c r="AK41" s="7"/>
-      <c r="AL41" s="7"/>
-      <c r="AM41" s="7"/>
-      <c r="AN41" s="1" t="s">
-        <v>110</v>
-      </c>
+      <c r="AMJ41" s="14"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
         <v>802</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C42" s="7" t="s">
         <v>111</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>112</v>
       </c>
       <c r="D42" s="7" t="s">
         <v>29</v>
@@ -5558,7 +5560,7 @@
         <v>29</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G42" s="7" t="s">
         <v>29</v>
@@ -5567,10 +5569,10 @@
         <v>29</v>
       </c>
       <c r="I42" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="J42" s="7" t="s">
         <v>113</v>
-      </c>
-      <c r="J42" s="7" t="s">
-        <v>114</v>
       </c>
       <c r="K42" s="7" t="s">
         <v>83</v>
@@ -5597,13 +5599,13 @@
         <v>29</v>
       </c>
       <c r="S42" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="T42" s="7" t="s">
         <v>29</v>
       </c>
       <c r="U42" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="V42" s="7" t="s">
         <v>29</v>
@@ -5618,13 +5620,13 @@
         <v>29</v>
       </c>
       <c r="Z42" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AA42" s="7" t="s">
         <v>29</v>
       </c>
       <c r="AB42" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AC42" s="7" t="s">
         <v>29</v>
@@ -5650,7 +5652,7 @@
       <c r="AJ42" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AK42" s="10" t="n">
+      <c r="AK42" s="9" t="n">
         <v>0</v>
       </c>
       <c r="AL42" s="1" t="n">
@@ -5660,7 +5662,7 @@
         <v>1</v>
       </c>
       <c r="AN42" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5668,28 +5670,28 @@
         <v>81</v>
       </c>
       <c r="B43" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C43" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D43" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E43" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F43" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G43" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H43" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I43" s="7" t="s">
         <v>119</v>
-      </c>
-      <c r="C43" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D43" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E43" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F43" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G43" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H43" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I43" s="7" t="s">
-        <v>120</v>
       </c>
       <c r="J43" s="7"/>
       <c r="K43" s="7"/>
@@ -5722,7 +5724,7 @@
       <c r="AL43" s="7"/>
       <c r="AM43" s="7"/>
       <c r="AN43" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5730,7 +5732,7 @@
         <v>842</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C44" s="1" t="n">
         <v>1</v>
@@ -5757,7 +5759,7 @@
         <v>0</v>
       </c>
       <c r="K44" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L44" s="1" t="n">
         <v>0</v>
@@ -5843,8 +5845,8 @@
       <c r="AM44" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AN44" s="9" t="s">
-        <v>123</v>
+      <c r="AN44" s="8" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5852,7 +5854,7 @@
         <v>85</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C45" s="1" t="n">
         <v>1</v>
@@ -5866,7 +5868,7 @@
       <c r="F45" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G45" s="10" t="n">
+      <c r="G45" s="9" t="n">
         <v>0</v>
       </c>
       <c r="H45" s="1" t="n">
@@ -5875,11 +5877,11 @@
       <c r="I45" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="J45" s="10" t="n">
+      <c r="J45" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K45" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L45" s="1" t="n">
         <v>0</v>
@@ -5887,7 +5889,7 @@
       <c r="M45" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="N45" s="10" t="n">
+      <c r="N45" s="9" t="n">
         <v>0</v>
       </c>
       <c r="O45" s="1" t="n">
@@ -5917,19 +5919,19 @@
       <c r="W45" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="X45" s="9" t="n">
+      <c r="X45" s="8" t="n">
         <v>0</v>
       </c>
       <c r="Y45" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Z45" s="10" t="n">
+      <c r="Z45" s="9" t="n">
         <v>0</v>
       </c>
       <c r="AA45" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AB45" s="10" t="n">
+      <c r="AB45" s="9" t="n">
         <v>0</v>
       </c>
       <c r="AC45" s="1" t="n">
@@ -5956,7 +5958,7 @@
       <c r="AJ45" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AK45" s="10" t="n">
+      <c r="AK45" s="9" t="n">
         <v>0</v>
       </c>
       <c r="AL45" s="1" t="n">
@@ -5966,7 +5968,7 @@
         <v>0</v>
       </c>
       <c r="AN45" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5974,7 +5976,7 @@
         <v>87</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C46" s="1" t="n">
         <v>0</v>
@@ -6001,7 +6003,7 @@
         <v>1</v>
       </c>
       <c r="K46" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L46" s="1" t="n">
         <v>1</v>
@@ -6039,7 +6041,7 @@
       <c r="W46" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="X46" s="9" t="n">
+      <c r="X46" s="8" t="n">
         <v>1</v>
       </c>
       <c r="Y46" s="1" t="n">
@@ -6088,7 +6090,7 @@
         <v>0</v>
       </c>
       <c r="AN46" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6096,40 +6098,40 @@
         <v>86</v>
       </c>
       <c r="B47" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C47" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F47" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I47" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L47" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="C47" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D47" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E47" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F47" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G47" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H47" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I47" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J47" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K47" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L47" s="7" t="s">
-        <v>129</v>
-      </c>
       <c r="M47" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N47" s="1" t="n">
         <v>0</v>
@@ -6137,7 +6139,7 @@
       <c r="O47" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P47" s="10" t="n">
+      <c r="P47" s="9" t="n">
         <v>0</v>
       </c>
       <c r="Q47" s="1" t="n">
@@ -6146,7 +6148,7 @@
       <c r="R47" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="S47" s="10" t="n">
+      <c r="S47" s="9" t="n">
         <v>0</v>
       </c>
       <c r="T47" s="1" t="n">
@@ -6161,7 +6163,7 @@
       <c r="W47" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="X47" s="10" t="n">
+      <c r="X47" s="9" t="n">
         <v>0</v>
       </c>
       <c r="Y47" s="1" t="n">
@@ -6182,7 +6184,7 @@
       <c r="AD47" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AE47" s="10" t="n">
+      <c r="AE47" s="9" t="n">
         <v>0</v>
       </c>
       <c r="AF47" s="1" t="n">
@@ -6191,7 +6193,7 @@
       <c r="AG47" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AH47" s="10" t="n">
+      <c r="AH47" s="9" t="n">
         <v>0</v>
       </c>
       <c r="AI47" s="1" t="n">
@@ -6210,15 +6212,15 @@
         <v>0</v>
       </c>
       <c r="AN47" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="n">
         <v>88</v>
       </c>
-      <c r="B48" s="14" t="s">
-        <v>131</v>
+      <c r="B48" s="15" t="s">
+        <v>130</v>
       </c>
       <c r="C48" s="1" t="n">
         <v>1</v>
@@ -6245,10 +6247,10 @@
         <v>0</v>
       </c>
       <c r="K48" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L48" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M48" s="7"/>
       <c r="N48" s="7"/>
@@ -6283,10 +6285,10 @@
         <v>882</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C49" s="7" t="s">
         <v>133</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>134</v>
       </c>
       <c r="D49" s="7"/>
       <c r="E49" s="7"/>
@@ -6308,7 +6310,7 @@
       <c r="O49" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P49" s="10" t="n">
+      <c r="P49" s="9" t="n">
         <v>0</v>
       </c>
       <c r="Q49" s="1" t="n">
@@ -6332,7 +6334,7 @@
       <c r="W49" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="X49" s="10" t="n">
+      <c r="X49" s="9" t="n">
         <v>0</v>
       </c>
       <c r="Y49" s="1" t="n">
@@ -6381,7 +6383,7 @@
         <v>0</v>
       </c>
       <c r="AN49" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6389,7 +6391,7 @@
         <v>89</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C50" s="1" t="n">
         <v>1</v>
@@ -6416,7 +6418,7 @@
         <v>0</v>
       </c>
       <c r="K50" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L50" s="1" t="n">
         <v>0</v>
@@ -6454,7 +6456,7 @@
       <c r="W50" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="X50" s="10" t="n">
+      <c r="X50" s="9" t="n">
         <v>0</v>
       </c>
       <c r="Y50" s="1" t="n">
@@ -6475,7 +6477,7 @@
       <c r="AD50" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AE50" s="10" t="n">
+      <c r="AE50" s="9" t="n">
         <v>0</v>
       </c>
       <c r="AF50" s="1" t="n">
@@ -6484,7 +6486,7 @@
       <c r="AG50" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AH50" s="10" t="n">
+      <c r="AH50" s="9" t="n">
         <v>0</v>
       </c>
       <c r="AI50" s="1" t="n">
@@ -6493,7 +6495,7 @@
       <c r="AJ50" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AK50" s="10" t="n">
+      <c r="AK50" s="9" t="n">
         <v>0</v>
       </c>
       <c r="AL50" s="1" t="n">
@@ -6503,7 +6505,7 @@
         <v>0</v>
       </c>
       <c r="AN50" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6511,7 +6513,7 @@
         <v>90</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C51" s="1" t="n">
         <v>1</v>
@@ -6615,7 +6617,7 @@
       <c r="AJ51" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AK51" s="10" t="n">
+      <c r="AK51" s="9" t="n">
         <v>0</v>
       </c>
       <c r="AL51" s="1" t="n">
@@ -6625,7 +6627,7 @@
         <v>1</v>
       </c>
       <c r="AN51" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6633,100 +6635,100 @@
         <v>93</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C52" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D52" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E52" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F52" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G52" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H52" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I52" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J52" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K52" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L52" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M52" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N52" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="O52" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P52" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q52" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R52" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S52" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="T52" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U52" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="V52" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W52" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="X52" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y52" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z52" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA52" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB52" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC52" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD52" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE52" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF52" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG52" s="7" t="s">
         <v>140</v>
-      </c>
-      <c r="C52" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D52" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E52" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F52" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G52" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H52" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I52" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J52" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="K52" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L52" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="M52" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N52" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="O52" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P52" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q52" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="R52" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="S52" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="T52" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="U52" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="V52" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="W52" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="X52" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y52" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z52" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA52" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB52" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC52" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD52" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE52" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="AF52" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG52" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="AH52" s="7"/>
       <c r="AI52" s="7"/>
@@ -6735,7 +6737,7 @@
       <c r="AL52" s="7"/>
       <c r="AM52" s="7"/>
       <c r="AN52" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6743,10 +6745,10 @@
         <v>932</v>
       </c>
       <c r="B53" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C53" s="7" t="s">
         <v>142</v>
-      </c>
-      <c r="C53" s="7" t="s">
-        <v>143</v>
       </c>
       <c r="D53" s="7"/>
       <c r="E53" s="7"/>
@@ -6804,7 +6806,7 @@
         <v>94</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C54" s="1" t="n">
         <v>1</v>
@@ -6831,7 +6833,7 @@
         <v>1</v>
       </c>
       <c r="K54" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L54" s="1" t="n">
         <v>1</v>
@@ -6918,7 +6920,7 @@
         <v>1</v>
       </c>
       <c r="AN54" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6926,7 +6928,7 @@
         <v>95</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C55" s="1" t="n">
         <v>1</v>
@@ -6982,7 +6984,7 @@
       <c r="T55" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="U55" s="15" t="n">
+      <c r="U55" s="16" t="n">
         <v>1</v>
       </c>
       <c r="V55" s="1" t="n">
@@ -7040,7 +7042,7 @@
         <v>1</v>
       </c>
       <c r="AN55" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7048,7 +7050,7 @@
         <v>96</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C56" s="1" t="n">
         <v>1</v>
@@ -7075,7 +7077,7 @@
         <v>0</v>
       </c>
       <c r="K56" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L56" s="1" t="n">
         <v>0</v>
@@ -7113,13 +7115,13 @@
       <c r="W56" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="X56" s="10" t="n">
+      <c r="X56" s="9" t="n">
         <v>0</v>
       </c>
       <c r="Y56" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Z56" s="10" t="n">
+      <c r="Z56" s="9" t="n">
         <v>0</v>
       </c>
       <c r="AA56" s="1" t="n">
@@ -7152,7 +7154,7 @@
       <c r="AJ56" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AK56" s="10" t="n">
+      <c r="AK56" s="9" t="n">
         <v>0</v>
       </c>
       <c r="AL56" s="1" t="n">
@@ -7162,7 +7164,7 @@
         <v>0</v>
       </c>
       <c r="AN56" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7170,7 +7172,7 @@
         <v>97</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C57" s="1" t="n">
         <v>1</v>
@@ -7197,7 +7199,7 @@
         <v>0</v>
       </c>
       <c r="K57" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L57" s="1" t="n">
         <v>0</v>
@@ -7284,7 +7286,7 @@
         <v>1</v>
       </c>
       <c r="AN57" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7292,7 +7294,7 @@
         <v>98</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C58" s="1" t="n">
         <v>1</v>
@@ -7369,7 +7371,7 @@
       <c r="AA58" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AB58" s="10" t="n">
+      <c r="AB58" s="9" t="n">
         <v>0</v>
       </c>
       <c r="AC58" s="1" t="n">
@@ -7387,7 +7389,7 @@
       <c r="AG58" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AH58" s="10" t="n">
+      <c r="AH58" s="9" t="n">
         <v>0</v>
       </c>
       <c r="AI58" s="1" t="n">
@@ -7406,17 +7408,17 @@
         <v>0</v>
       </c>
       <c r="AN58" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B75" s="5"/>
       <c r="C75" s="5"/>

</xml_diff>